<commit_message>
Update calculation of lift and leverage
</commit_message>
<xml_diff>
--- a/Lattice.xlsx
+++ b/Lattice.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/situsnow/git/OpusMiner_SDRD/opus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/situsnow/git/OpusMiner_SDRD/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1640" yWindow="520" windowWidth="23060" windowHeight="14020" tabRatio="500"/>
+    <workbookView xWindow="8240" yWindow="640" windowWidth="23060" windowHeight="14020" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="104">
   <si>
     <t>null</t>
   </si>
@@ -488,13 +489,64 @@
   </si>
   <si>
     <t>dbeac</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>EDIBLE</t>
+  </si>
+  <si>
+    <t>POISONOUS</t>
+  </si>
+  <si>
+    <t>!A</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>field2 = CONVEX</t>
+  </si>
+  <si>
+    <t>!B</t>
+  </si>
+  <si>
+    <t>field2 != CONVEX</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>EDIBLE/field2 = CONVEX</t>
+  </si>
+  <si>
+    <t>Lift</t>
+  </si>
+  <si>
+    <t>Leverage</t>
+  </si>
+  <si>
+    <t>field6 = NONE</t>
+  </si>
+  <si>
+    <t>EDIBLE/field6 = NONE</t>
+  </si>
+  <si>
+    <t>field9 = BROAD</t>
+  </si>
+  <si>
+    <t>EDIBLE/field9 = BROAD</t>
+  </si>
+  <si>
+    <t>field6 = NONE/field9 = BROAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -533,6 +585,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -560,7 +620,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -568,16 +628,125 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="L11" sqref="K1:L11"/>
     </sheetView>
   </sheetViews>
@@ -1373,4 +1542,288 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1">
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2">
+        <v>4488</v>
+      </c>
+      <c r="C2">
+        <f>B2/$B$1</f>
+        <v>0.53326996197718635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3">
+        <v>3928</v>
+      </c>
+      <c r="C3">
+        <f>B3/$B$1</f>
+        <v>0.46673003802281371</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="8">
+        <v>3796</v>
+      </c>
+      <c r="C5" s="9">
+        <f>B5/$B$1</f>
+        <v>0.45104562737642584</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3928</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2404</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2084</v>
+      </c>
+      <c r="C6" s="12">
+        <f>B6/$B$1</f>
+        <v>0.24762357414448669</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2084</v>
+      </c>
+      <c r="I6" s="5">
+        <f>G6+H6</f>
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <f>H5+H6</f>
+        <v>4488</v>
+      </c>
+      <c r="I7" s="5">
+        <f>G5+H5+G6+H6</f>
+        <v>8416</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="11">
+        <f>C6/(C5*$C$2)</f>
+        <v>1.0294953502044557</v>
+      </c>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="14">
+        <f>C6-C5*$C$2</f>
+        <v>7.0944895834839095E-3</v>
+      </c>
+      <c r="C9" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3808</v>
+      </c>
+      <c r="C12" s="9">
+        <f>B12/$B$1</f>
+        <v>0.45247148288973382</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="11">
+        <v>3688</v>
+      </c>
+      <c r="C13" s="12">
+        <f>B13/$B$1</f>
+        <v>0.43821292775665399</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14">
+        <v>3544</v>
+      </c>
+      <c r="G14">
+        <f>F14/B1</f>
+        <v>0.42110266159695819</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="11">
+        <f>C13/(C12*$C$2)</f>
+        <v>1.8161296604203176</v>
+      </c>
+      <c r="C15" s="12"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="14">
+        <f>C13-C12*$C$2</f>
+        <v>0.1969234772802845</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="E16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16">
+        <f>G14/C12*C19</f>
+        <v>0.65023205099530301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17">
+        <f>G14-C12*C19</f>
+        <v>0.10497477193540466</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19" s="8">
+        <v>5880</v>
+      </c>
+      <c r="C19" s="9">
+        <f>B19/$B$1</f>
+        <v>0.6986692015209125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20" s="11">
+        <v>4176</v>
+      </c>
+      <c r="C20" s="12">
+        <f>B20/$B$1</f>
+        <v>0.49619771863117873</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="10"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" s="11">
+        <f>C20/(C19*$C$2)</f>
+        <v>1.3317908981774529</v>
+      </c>
+      <c r="C22" s="12"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="14">
+        <f>C20-C19*$C$2</f>
+        <v>0.1236184201014906</v>
+      </c>
+      <c r="C23" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>